<commit_message>
add database and questions in EntwurfET.xlsx
on sheet 3
</commit_message>
<xml_diff>
--- a/EntwurfET.xlsx
+++ b/EntwurfET.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-2370" yWindow="15" windowWidth="27795" windowHeight="13350" activeTab="1"/>
+    <workbookView xWindow="-2370" yWindow="15" windowWidth="27795" windowHeight="13350" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="170">
   <si>
     <t>Kapital vorhanden</t>
   </si>
@@ -424,6 +424,111 @@
   </si>
   <si>
     <t>G (ExFB) UE</t>
+  </si>
+  <si>
+    <t>Mindestkapital nötig?</t>
+  </si>
+  <si>
+    <t>sehr</t>
+  </si>
+  <si>
+    <t>mittel</t>
+  </si>
+  <si>
+    <t>wenig</t>
+  </si>
+  <si>
+    <t>wie wichtig ist:</t>
+  </si>
+  <si>
+    <t>Haftungsbeschränkung</t>
+  </si>
+  <si>
+    <t>Breiter Entscheidungsspielraum</t>
+  </si>
+  <si>
+    <t>Wenig Formalitäten</t>
+  </si>
+  <si>
+    <t>Hohes Ansehen, Kreditwürdigkeit duch persönliche Haftung</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>EK</t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>PartG</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>GMbH &amp; Co. KG</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>eG</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>mögl.</t>
+  </si>
+  <si>
+    <t>z.T.</t>
+  </si>
+  <si>
+    <t>deutsche firma?</t>
+  </si>
+  <si>
+    <t>KGaA</t>
+  </si>
+  <si>
+    <t>dt?</t>
+  </si>
+  <si>
+    <t>sp.z.o.o.</t>
+  </si>
+  <si>
+    <t>z.t.</t>
+  </si>
+  <si>
+    <t>pcl by s</t>
+  </si>
+  <si>
+    <t>plc</t>
+  </si>
+  <si>
+    <t>mögl</t>
+  </si>
+  <si>
+    <t>Eintrag Handelsregister</t>
+  </si>
+  <si>
+    <t>gemeinnützig?</t>
+  </si>
+  <si>
+    <t>gemeinnützig</t>
+  </si>
+  <si>
+    <t>e.V.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stiftung </t>
+  </si>
+  <si>
+    <t>cic</t>
+  </si>
+  <si>
+    <t>micro</t>
   </si>
 </sst>
 </file>
@@ -492,7 +597,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -539,9 +644,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -579,7 +684,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -651,7 +756,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -831,7 +936,7 @@
       <selection activeCell="B24" sqref="B24:Q42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="32.140625" customWidth="1"/>
   </cols>
@@ -1071,21 +1176,21 @@
   </sheetPr>
   <dimension ref="B4:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="3.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
     <col min="8" max="8" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" width="2.5703125" customWidth="1"/>
-    <col min="10" max="10" width="2.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="38.85546875" customWidth="1"/>
     <col min="12" max="12" width="44.28515625" customWidth="1"/>
     <col min="13" max="13" width="8.5703125" customWidth="1"/>
@@ -1842,12 +1947,603 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C2:U24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="54.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>145</v>
+      </c>
+      <c r="E15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" t="s">
+        <v>147</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" t="s">
+        <v>148</v>
+      </c>
+      <c r="I15" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" t="s">
+        <v>149</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" t="s">
+        <v>150</v>
+      </c>
+      <c r="N15" t="s">
+        <v>15</v>
+      </c>
+      <c r="O15" t="s">
+        <v>151</v>
+      </c>
+      <c r="P15" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>161</v>
+      </c>
+      <c r="R15" t="s">
+        <v>166</v>
+      </c>
+      <c r="S15" t="s">
+        <v>167</v>
+      </c>
+      <c r="T15" t="s">
+        <v>168</v>
+      </c>
+      <c r="U15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>144</v>
+      </c>
+      <c r="E17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" t="s">
+        <v>152</v>
+      </c>
+      <c r="J17" t="s">
+        <v>152</v>
+      </c>
+      <c r="K17" t="s">
+        <v>152</v>
+      </c>
+      <c r="L17" t="s">
+        <v>152</v>
+      </c>
+      <c r="M17" t="s">
+        <v>152</v>
+      </c>
+      <c r="N17" t="s">
+        <v>152</v>
+      </c>
+      <c r="O17" t="s">
+        <v>152</v>
+      </c>
+      <c r="P17" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>152</v>
+      </c>
+      <c r="R17" t="s">
+        <v>144</v>
+      </c>
+      <c r="S17" t="s">
+        <v>144</v>
+      </c>
+      <c r="T17" t="s">
+        <v>144</v>
+      </c>
+      <c r="U17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" t="s">
+        <v>153</v>
+      </c>
+      <c r="G18" t="s">
+        <v>144</v>
+      </c>
+      <c r="H18" t="s">
+        <v>154</v>
+      </c>
+      <c r="I18" t="s">
+        <v>152</v>
+      </c>
+      <c r="J18" t="s">
+        <v>152</v>
+      </c>
+      <c r="K18" t="s">
+        <v>152</v>
+      </c>
+      <c r="L18" t="s">
+        <v>159</v>
+      </c>
+      <c r="M18" t="s">
+        <v>152</v>
+      </c>
+      <c r="N18" t="s">
+        <v>152</v>
+      </c>
+      <c r="O18" t="s">
+        <v>152</v>
+      </c>
+      <c r="P18" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>152</v>
+      </c>
+      <c r="R18" t="s">
+        <v>152</v>
+      </c>
+      <c r="S18" t="s">
+        <v>144</v>
+      </c>
+      <c r="T18" t="s">
+        <v>152</v>
+      </c>
+      <c r="U18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" t="s">
+        <v>152</v>
+      </c>
+      <c r="E19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" t="s">
+        <v>152</v>
+      </c>
+      <c r="J19" t="s">
+        <v>152</v>
+      </c>
+      <c r="K19" t="s">
+        <v>144</v>
+      </c>
+      <c r="L19" t="s">
+        <v>144</v>
+      </c>
+      <c r="M19" t="s">
+        <v>144</v>
+      </c>
+      <c r="N19" t="s">
+        <v>144</v>
+      </c>
+      <c r="O19" t="s">
+        <v>144</v>
+      </c>
+      <c r="P19" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>152</v>
+      </c>
+      <c r="R19" t="s">
+        <v>152</v>
+      </c>
+      <c r="S19" t="s">
+        <v>152</v>
+      </c>
+      <c r="T19" t="s">
+        <v>152</v>
+      </c>
+      <c r="U19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>142</v>
+      </c>
+      <c r="D20" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F20" t="s">
+        <v>152</v>
+      </c>
+      <c r="G20" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" t="s">
+        <v>144</v>
+      </c>
+      <c r="J20" t="s">
+        <v>144</v>
+      </c>
+      <c r="K20" t="s">
+        <v>152</v>
+      </c>
+      <c r="L20" t="s">
+        <v>152</v>
+      </c>
+      <c r="M20" t="s">
+        <v>152</v>
+      </c>
+      <c r="N20" t="s">
+        <v>144</v>
+      </c>
+      <c r="O20" t="s">
+        <v>144</v>
+      </c>
+      <c r="P20" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>152</v>
+      </c>
+      <c r="R20" t="s">
+        <v>144</v>
+      </c>
+      <c r="S20" t="s">
+        <v>144</v>
+      </c>
+      <c r="T20" t="s">
+        <v>144</v>
+      </c>
+      <c r="U20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+      <c r="E21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" t="s">
+        <v>152</v>
+      </c>
+      <c r="G21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" t="s">
+        <v>152</v>
+      </c>
+      <c r="I21" t="s">
+        <v>152</v>
+      </c>
+      <c r="J21" t="s">
+        <v>152</v>
+      </c>
+      <c r="K21" t="s">
+        <v>152</v>
+      </c>
+      <c r="L21" t="s">
+        <v>152</v>
+      </c>
+      <c r="M21" t="s">
+        <v>152</v>
+      </c>
+      <c r="N21" t="s">
+        <v>152</v>
+      </c>
+      <c r="O21" t="s">
+        <v>152</v>
+      </c>
+      <c r="P21" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>152</v>
+      </c>
+      <c r="R21" t="s">
+        <v>144</v>
+      </c>
+      <c r="S21" t="s">
+        <v>144</v>
+      </c>
+      <c r="T21" t="s">
+        <v>144</v>
+      </c>
+      <c r="U21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>152</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" t="s">
+        <v>152</v>
+      </c>
+      <c r="H22" t="s">
+        <v>152</v>
+      </c>
+      <c r="I22" t="s">
+        <v>152</v>
+      </c>
+      <c r="J22" t="s">
+        <v>144</v>
+      </c>
+      <c r="K22" t="s">
+        <v>144</v>
+      </c>
+      <c r="L22" t="s">
+        <v>144</v>
+      </c>
+      <c r="M22" t="s">
+        <v>144</v>
+      </c>
+      <c r="N22" t="s">
+        <v>144</v>
+      </c>
+      <c r="O22" t="s">
+        <v>144</v>
+      </c>
+      <c r="P22" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>144</v>
+      </c>
+      <c r="R22" t="s">
+        <v>144</v>
+      </c>
+      <c r="S22" t="s">
+        <v>144</v>
+      </c>
+      <c r="T22" t="s">
+        <v>144</v>
+      </c>
+      <c r="U22" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
+        <v>152</v>
+      </c>
+      <c r="E23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" t="s">
+        <v>152</v>
+      </c>
+      <c r="G23" t="s">
+        <v>152</v>
+      </c>
+      <c r="H23" t="s">
+        <v>152</v>
+      </c>
+      <c r="I23" t="s">
+        <v>152</v>
+      </c>
+      <c r="J23" t="s">
+        <v>152</v>
+      </c>
+      <c r="K23" t="s">
+        <v>152</v>
+      </c>
+      <c r="L23" t="s">
+        <v>144</v>
+      </c>
+      <c r="M23" t="s">
+        <v>152</v>
+      </c>
+      <c r="N23" t="s">
+        <v>152</v>
+      </c>
+      <c r="O23" t="s">
+        <v>152</v>
+      </c>
+      <c r="P23" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>162</v>
+      </c>
+      <c r="R23" t="s">
+        <v>152</v>
+      </c>
+      <c r="S23" t="s">
+        <v>152</v>
+      </c>
+      <c r="T23" t="s">
+        <v>144</v>
+      </c>
+      <c r="U23" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>165</v>
+      </c>
+      <c r="D24" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" t="s">
+        <v>144</v>
+      </c>
+      <c r="F24" t="s">
+        <v>144</v>
+      </c>
+      <c r="G24" t="s">
+        <v>144</v>
+      </c>
+      <c r="H24" t="s">
+        <v>144</v>
+      </c>
+      <c r="I24" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" t="s">
+        <v>144</v>
+      </c>
+      <c r="K24" t="s">
+        <v>144</v>
+      </c>
+      <c r="L24" t="s">
+        <v>144</v>
+      </c>
+      <c r="M24" t="s">
+        <v>144</v>
+      </c>
+      <c r="N24" t="s">
+        <v>144</v>
+      </c>
+      <c r="O24" t="s">
+        <v>144</v>
+      </c>
+      <c r="P24" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>144</v>
+      </c>
+      <c r="R24" t="s">
+        <v>152</v>
+      </c>
+      <c r="S24" t="s">
+        <v>152</v>
+      </c>
+      <c r="T24" t="s">
+        <v>144</v>
+      </c>
+      <c r="U24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>